<commit_message>
added backend functionality tasks tracker documentation
</commit_message>
<xml_diff>
--- a/files/documentation/Backend Functionalities.xlsx
+++ b/files/documentation/Backend Functionalities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALEX PROGRAMARE\SwapIt\files\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FEF45B6-7BCB-42DC-82AB-3DDD3B9999A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC1C0C42-B201-4DFB-B0CB-896AB9C6A48F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Functionality</t>
   </si>
@@ -117,16 +117,27 @@
   </si>
   <si>
     <t>Store User Profile picture</t>
+  </si>
+  <si>
+    <t>Add Data for testing (50 different users with lots of 
+conversations, products, etc)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -179,7 +190,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -189,6 +200,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -469,10 +481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -738,6 +750,15 @@
       </c>
       <c r="C30" s="3"/>
     </row>
+    <row r="31" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>7</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C31" s="5"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added product update functionality + a lot of refactoring
</commit_message>
<xml_diff>
--- a/files/documentation/Backend Functionalities.xlsx
+++ b/files/documentation/Backend Functionalities.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALEX PROGRAMARE\SwapIt\files\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC1C0C42-B201-4DFB-B0CB-896AB9C6A48F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5F92A59-99F3-4892-A01B-6EA2F6DB4567}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-7290" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Functionality</t>
   </si>
@@ -100,9 +100,6 @@
   </si>
   <si>
     <t>Update Product</t>
-  </si>
-  <si>
-    <t>Like product (Increase popularity)</t>
   </si>
   <si>
     <t>Recommend products based on previous preferences
@@ -121,13 +118,21 @@
   <si>
     <t>Add Data for testing (50 different users with lots of 
 conversations, products, etc)</t>
+  </si>
+  <si>
+    <t>Like product (Increase popularity) and identify 
+if the user has liked this product or not</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use @Transactional for methods that need more than one 
+Db interaction </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,6 +143,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -190,7 +202,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -201,6 +213,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -481,16 +494,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" customWidth="1"/>
-    <col min="2" max="2" width="45.109375" customWidth="1"/>
+    <col min="2" max="2" width="54.6640625" customWidth="1"/>
     <col min="3" max="3" width="21.44140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -653,14 +666,14 @@
       <c r="B18" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="4"/>
-    </row>
-    <row r="19" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C18" s="6"/>
+    </row>
+    <row r="19" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" t="s">
-        <v>25</v>
+      <c r="B19" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="C19" s="4"/>
     </row>
@@ -669,7 +682,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C20" s="4"/>
     </row>
@@ -678,7 +691,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C21" s="4"/>
     </row>
@@ -687,7 +700,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C22" s="4"/>
     </row>
@@ -746,7 +759,7 @@
         <v>6</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C30" s="3"/>
     </row>
@@ -755,9 +768,18 @@
         <v>7</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C31" s="5"/>
+    </row>
+    <row r="32" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>8</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C32" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added product like functionality + separated user details retrieval from the products details of the user
</commit_message>
<xml_diff>
--- a/files/documentation/Backend Functionalities.xlsx
+++ b/files/documentation/Backend Functionalities.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALEX PROGRAMARE\SwapIt\files\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5F92A59-99F3-4892-A01B-6EA2F6DB4567}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACE197EF-1806-4861-9472-37AB9024ABFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-7290" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32415" yWindow="-5865" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Functionality</t>
   </si>
@@ -126,6 +126,12 @@
   <si>
     <t xml:space="preserve">Use @Transactional for methods that need more than one 
 Db interaction </t>
+  </si>
+  <si>
+    <t>Delete Product</t>
+  </si>
+  <si>
+    <t>Ban User</t>
   </si>
 </sst>
 </file>
@@ -175,7 +181,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -198,11 +204,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -214,6 +233,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -494,10 +514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -675,7 +695,7 @@
       <c r="B19" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="4"/>
+      <c r="C19" s="3"/>
     </row>
     <row r="20" spans="1:3" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20">
@@ -704,82 +724,100 @@
       </c>
       <c r="C22" s="4"/>
     </row>
+    <row r="23" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" s="7"/>
+    </row>
     <row r="24" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="1" t="s">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24" s="4"/>
+    </row>
+    <row r="26" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B26" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25">
-        <v>1</v>
-      </c>
-      <c r="B25" t="s">
-        <v>19</v>
-      </c>
-      <c r="C25" s="3"/>
-    </row>
-    <row r="26" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26">
-        <v>2</v>
-      </c>
-      <c r="B26" t="s">
-        <v>20</v>
-      </c>
-      <c r="C26" s="3"/>
     </row>
     <row r="27" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B27" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C27" s="3"/>
     </row>
     <row r="28" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B28" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C28" s="3"/>
     </row>
     <row r="29" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29">
+        <v>3</v>
+      </c>
+      <c r="B29" t="s">
+        <v>21</v>
+      </c>
+      <c r="C29" s="3"/>
+    </row>
+    <row r="30" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>4</v>
+      </c>
+      <c r="B30" t="s">
+        <v>22</v>
+      </c>
+      <c r="C30" s="3"/>
+    </row>
+    <row r="31" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31">
         <v>5</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B31" t="s">
         <v>23</v>
       </c>
-      <c r="C29" s="3"/>
-    </row>
-    <row r="30" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30">
-        <v>6</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C30" s="3"/>
-    </row>
-    <row r="31" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31">
-        <v>7</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C31" s="5"/>
+      <c r="C31" s="3"/>
     </row>
     <row r="32" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32">
+        <v>6</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C32" s="3"/>
+    </row>
+    <row r="33" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>7</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C33" s="5"/>
+    </row>
+    <row r="34" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34">
         <v>8</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B34" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C32" s="3"/>
+      <c r="C34" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added batch processing of data + product recommendations
</commit_message>
<xml_diff>
--- a/files/documentation/Backend Functionalities.xlsx
+++ b/files/documentation/Backend Functionalities.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALEX PROGRAMARE\SwapIt\files\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACE197EF-1806-4861-9472-37AB9024ABFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E261DDA-21DA-429F-9B98-B35EC7B4A19E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32415" yWindow="-5865" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-7290" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Functionality</t>
   </si>
@@ -132,13 +132,23 @@
   </si>
   <si>
     <t>Ban User</t>
+  </si>
+  <si>
+    <t>Process data in batches</t>
+  </si>
+  <si>
+    <t>Recommend products Random sorted by popularity, newest
+random</t>
+  </si>
+  <si>
+    <t>Enhance user login methods, etc</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -156,6 +166,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -221,7 +238,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -234,6 +251,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -514,10 +532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -742,82 +760,112 @@
       </c>
       <c r="C24" s="4"/>
     </row>
+    <row r="25" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C25" s="3"/>
+    </row>
     <row r="26" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="1" t="s">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26" s="4"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C27" s="8"/>
+    </row>
+    <row r="29" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B29" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27">
-        <v>1</v>
-      </c>
-      <c r="B27" t="s">
-        <v>19</v>
-      </c>
-      <c r="C27" s="3"/>
-    </row>
-    <row r="28" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28">
-        <v>2</v>
-      </c>
-      <c r="B28" t="s">
-        <v>20</v>
-      </c>
-      <c r="C28" s="3"/>
-    </row>
-    <row r="29" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29">
-        <v>3</v>
-      </c>
-      <c r="B29" t="s">
-        <v>21</v>
-      </c>
-      <c r="C29" s="3"/>
     </row>
     <row r="30" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B30" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C30" s="3"/>
     </row>
     <row r="31" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31">
+        <v>2</v>
+      </c>
+      <c r="B31" t="s">
+        <v>20</v>
+      </c>
+      <c r="C31" s="3"/>
+    </row>
+    <row r="32" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>3</v>
+      </c>
+      <c r="B32" t="s">
+        <v>21</v>
+      </c>
+      <c r="C32" s="3"/>
+    </row>
+    <row r="33" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>4</v>
+      </c>
+      <c r="B33" t="s">
+        <v>22</v>
+      </c>
+      <c r="C33" s="3"/>
+    </row>
+    <row r="34" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34">
         <v>5</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B34" t="s">
         <v>23</v>
       </c>
-      <c r="C31" s="3"/>
-    </row>
-    <row r="32" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32">
+      <c r="C34" s="3"/>
+    </row>
+    <row r="35" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35">
         <v>6</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B35" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C32" s="3"/>
-    </row>
-    <row r="33" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33">
+      <c r="C35" s="3"/>
+    </row>
+    <row r="36" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36">
         <v>7</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B36" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C33" s="5"/>
-    </row>
-    <row r="34" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34">
+      <c r="C36" s="5"/>
+    </row>
+    <row r="37" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37">
         <v>8</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B37" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C34" s="3"/>
+      <c r="C37" s="3"/>
+    </row>
+    <row r="38" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A38">
+        <v>9</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C38" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
enhanced registration process with email code registration + user image
</commit_message>
<xml_diff>
--- a/files/documentation/Backend Functionalities.xlsx
+++ b/files/documentation/Backend Functionalities.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALEX PROGRAMARE\SwapIt\files\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E261DDA-21DA-429F-9B98-B35EC7B4A19E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DD22289-F738-4779-8E72-677E3FFD462B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-7290" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>Functionality</t>
   </si>
@@ -142,6 +142,10 @@
   </si>
   <si>
     <t>Enhance user login methods, etc</t>
+  </si>
+  <si>
+    <t>Make chron microservice with delete every 15 minutes of
+unused codes longer than 15 minutes</t>
   </si>
 </sst>
 </file>
@@ -238,7 +242,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -252,6 +256,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -532,10 +537,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C38"/>
+  <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -731,7 +736,7 @@
       <c r="B21" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="4"/>
+      <c r="C21" s="3"/>
     </row>
     <row r="22" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22">
@@ -740,7 +745,7 @@
       <c r="B22" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="4"/>
+      <c r="C22" s="3"/>
     </row>
     <row r="23" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23">
@@ -778,94 +783,103 @@
       </c>
       <c r="C26" s="4"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C27" s="8"/>
-    </row>
-    <row r="29" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="1" t="s">
+    <row r="27" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C27" s="9"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C28" s="8"/>
+    </row>
+    <row r="30" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B30" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30">
-        <v>1</v>
-      </c>
-      <c r="B30" t="s">
-        <v>19</v>
-      </c>
-      <c r="C30" s="3"/>
     </row>
     <row r="31" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B31" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C31" s="3"/>
     </row>
     <row r="32" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B32" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C32" s="3"/>
     </row>
     <row r="33" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B33" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C33" s="3"/>
     </row>
     <row r="34" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34">
+        <v>4</v>
+      </c>
+      <c r="B34" t="s">
+        <v>22</v>
+      </c>
+      <c r="C34" s="3"/>
+    </row>
+    <row r="35" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35">
         <v>5</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B35" t="s">
         <v>23</v>
-      </c>
-      <c r="C34" s="3"/>
-    </row>
-    <row r="35" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35">
-        <v>6</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="C35" s="3"/>
     </row>
     <row r="36" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C36" s="5"/>
+        <v>26</v>
+      </c>
+      <c r="C36" s="3"/>
     </row>
     <row r="37" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37">
+        <v>7</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C37" s="5"/>
+    </row>
+    <row r="38" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A38">
         <v>8</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B38" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C37" s="3"/>
-    </row>
-    <row r="38" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38">
+      <c r="C38" s="3"/>
+    </row>
+    <row r="39" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39">
         <v>9</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B39" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C38" s="3"/>
+      <c r="C39" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added Exception handling with custom error codes for better FE control over errors
</commit_message>
<xml_diff>
--- a/files/documentation/Backend Functionalities.xlsx
+++ b/files/documentation/Backend Functionalities.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALEX PROGRAMARE\SwapIt\files\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F059C4D0-6964-44F5-A590-9D93F7E07E6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77DCF6F8-CD0B-41A6-A1E6-18F809D1ED5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32850" yWindow="-5430" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-7290" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>Functionality</t>
   </si>
@@ -146,6 +146,9 @@
   <si>
     <t>Make chron microservice with delete every 15 minutes of
 unused codes longer than 15 minutes</t>
+  </si>
+  <si>
+    <t>Exceptions handling for better FE control of errors</t>
   </si>
 </sst>
 </file>
@@ -537,10 +540,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C39"/>
+  <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -881,6 +884,15 @@
       </c>
       <c r="C39" s="3"/>
     </row>
+    <row r="40" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40">
+        <v>10</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C40" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
improved security a lot
</commit_message>
<xml_diff>
--- a/files/documentation/Backend Functionalities.xlsx
+++ b/files/documentation/Backend Functionalities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALEX PROGRAMARE\SwapIt\files\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77DCF6F8-CD0B-41A6-A1E6-18F809D1ED5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{443A0C0D-F309-4D60-A4BF-067BCF72B9AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-7290" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -542,8 +542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Added delete product functionality
</commit_message>
<xml_diff>
--- a/files/documentation/Backend Functionalities.xlsx
+++ b/files/documentation/Backend Functionalities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALEX PROGRAMARE\SwapIt\files\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{443A0C0D-F309-4D60-A4BF-067BCF72B9AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9A44069-B517-4835-B29A-1F87A49F54FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-7290" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -257,9 +257,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -543,7 +543,7 @@
   <dimension ref="A1:C40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -757,7 +757,7 @@
       <c r="B23" t="s">
         <v>32</v>
       </c>
-      <c r="C23" s="7"/>
+      <c r="C23" s="9"/>
     </row>
     <row r="24" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24">
@@ -793,10 +793,10 @@
       <c r="B27" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C27" s="9"/>
+      <c r="C27" s="8"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C28" s="8"/>
+      <c r="C28" s="7"/>
     </row>
     <row r="30" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B30" s="1" t="s">

</xml_diff>

<commit_message>
Finished Login/SignUp/Forgot Password functionality in UI
</commit_message>
<xml_diff>
--- a/files/documentation/Backend Functionalities.xlsx
+++ b/files/documentation/Backend Functionalities.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALEX PROGRAMARE\SwapIt\files\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83783746-2CB0-487B-89B9-36D0B0E49AB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD6A7473-C013-462A-B1A9-93C5F794CFF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-7290" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>Functionality</t>
   </si>
@@ -149,6 +149,12 @@
   </si>
   <si>
     <t>Exceptions handling for better FE control of errors</t>
+  </si>
+  <si>
+    <t>Reset Passwod functionality</t>
+  </si>
+  <si>
+    <t>Make swagger work with jwtToken header</t>
   </si>
 </sst>
 </file>
@@ -245,7 +251,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -260,6 +266,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -540,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C40"/>
+  <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -796,102 +803,120 @@
       <c r="C27" s="8"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C28" s="7"/>
-    </row>
-    <row r="30" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="1" t="s">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C28" s="10"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C29" s="7"/>
+    </row>
+    <row r="31" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B31" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31">
-        <v>1</v>
-      </c>
-      <c r="B31" t="s">
-        <v>19</v>
-      </c>
-      <c r="C31" s="3"/>
     </row>
     <row r="32" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B32" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C32" s="3"/>
     </row>
     <row r="33" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B33" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C33" s="3"/>
     </row>
     <row r="34" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B34" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C34" s="3"/>
     </row>
     <row r="35" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35">
+        <v>4</v>
+      </c>
+      <c r="B35" t="s">
+        <v>22</v>
+      </c>
+      <c r="C35" s="3"/>
+    </row>
+    <row r="36" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36">
         <v>5</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B36" t="s">
         <v>23</v>
-      </c>
-      <c r="C35" s="3"/>
-    </row>
-    <row r="36" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36">
-        <v>6</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="C36" s="3"/>
     </row>
     <row r="37" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C37" s="5"/>
+        <v>26</v>
+      </c>
+      <c r="C37" s="3"/>
     </row>
     <row r="38" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38">
+        <v>7</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C38" s="5"/>
+    </row>
+    <row r="39" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39">
         <v>8</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B39" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="C38" s="3"/>
-    </row>
-    <row r="39" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39">
-        <v>9</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>34</v>
       </c>
       <c r="C39" s="3"/>
     </row>
     <row r="40" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40">
+        <v>9</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C40" s="3"/>
+    </row>
+    <row r="41" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41">
         <v>10</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B41" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C40" s="3"/>
+      <c r="C41" s="3"/>
+    </row>
+    <row r="42" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A42">
+        <v>11</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C42" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added user actions log - backend
</commit_message>
<xml_diff>
--- a/files/documentation/Backend Functionalities.xlsx
+++ b/files/documentation/Backend Functionalities.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALEX PROGRAMARE\SwapIt\files\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD6A7473-C013-462A-B1A9-93C5F794CFF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3A6E873-D9D5-428C-91E3-B7A261A80AA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-7290" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>Functionality</t>
   </si>
@@ -155,6 +155,9 @@
   </si>
   <si>
     <t>Make swagger work with jwtToken header</t>
+  </si>
+  <si>
+    <t>Add users actions logs</t>
   </si>
 </sst>
 </file>
@@ -266,7 +269,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -547,10 +552,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C42"/>
+  <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -802,121 +807,130 @@
       </c>
       <c r="C27" s="8"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C28" s="10"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C29" s="7"/>
-    </row>
-    <row r="31" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="1" t="s">
+      <c r="C28" s="8"/>
+    </row>
+    <row r="29" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C29" s="8"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C30" s="7"/>
+    </row>
+    <row r="32" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B32" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32">
-        <v>1</v>
-      </c>
-      <c r="B32" t="s">
-        <v>19</v>
-      </c>
-      <c r="C32" s="3"/>
     </row>
     <row r="33" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B33" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C33" s="3"/>
     </row>
     <row r="34" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B34" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C34" s="3"/>
     </row>
     <row r="35" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B35" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C35" s="3"/>
     </row>
     <row r="36" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36">
+        <v>4</v>
+      </c>
+      <c r="B36" t="s">
+        <v>22</v>
+      </c>
+      <c r="C36" s="3"/>
+    </row>
+    <row r="37" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37">
         <v>5</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B37" t="s">
         <v>23</v>
-      </c>
-      <c r="C36" s="3"/>
-    </row>
-    <row r="37" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37">
-        <v>6</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="C37" s="3"/>
     </row>
     <row r="38" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C38" s="5"/>
+        <v>26</v>
+      </c>
+      <c r="C38" s="3"/>
     </row>
     <row r="39" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39">
+        <v>7</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C39" s="5"/>
+    </row>
+    <row r="40" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40">
         <v>8</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B40" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="C39" s="3"/>
-    </row>
-    <row r="40" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40">
-        <v>9</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>34</v>
       </c>
       <c r="C40" s="3"/>
     </row>
     <row r="41" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C41" s="3"/>
     </row>
     <row r="42" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42">
+        <v>10</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C42" s="3"/>
+    </row>
+    <row r="43" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43">
         <v>11</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B43" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C42" s="3"/>
+      <c r="C43" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>